<commit_message>
Updated_Format_1 (Text Wrapper+Coloana B mai mica)
</commit_message>
<xml_diff>
--- a/scripts/filler_sentences/output/wsd_1.xlsx
+++ b/scripts/filler_sentences/output/wsd_1.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
-    <t>Numele și Prenumele:</t>
+    <t xml:space="preserve">  Numele și Prenumele:</t>
   </si>
   <si>
     <t xml:space="preserve">  &lt;introduceți numele aici&gt;</t>
@@ -162,7 +162,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF808080"/>
+      <color rgb="FFE3E3E3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -274,22 +276,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,7 +594,7 @@
   <sheetFormatPr defaultRowHeight="26" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="250.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="200.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -635,6 +637,9 @@
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" ht="26" customHeight="1">
+      <c r="A7" s="2">
+        <v>10</v>
+      </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:2" ht="26" customHeight="1">
@@ -682,6 +687,9 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="26" customHeight="1">
+      <c r="A19" s="2">
+        <v>9</v>
+      </c>
       <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:2" ht="26" customHeight="1">
@@ -729,6 +737,9 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="26" customHeight="1">
+      <c r="A31" s="2">
+        <v>3</v>
+      </c>
       <c r="B31" s="11" t="s">
         <v>12</v>
       </c>
@@ -786,6 +797,9 @@
       <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:2" ht="26" customHeight="1">
+      <c r="A43" s="2">
+        <v>10</v>
+      </c>
       <c r="B43" s="9"/>
     </row>
     <row r="44" spans="1:2" ht="26" customHeight="1">
@@ -831,6 +845,9 @@
       <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" ht="26" customHeight="1">
+      <c r="A55" s="2">
+        <v>10</v>
+      </c>
       <c r="B55" s="9"/>
     </row>
     <row r="56" spans="1:2" ht="26" customHeight="1">
@@ -876,6 +893,9 @@
       <c r="B66" s="8"/>
     </row>
     <row r="67" spans="1:2" ht="26" customHeight="1">
+      <c r="A67" s="2">
+        <v>10</v>
+      </c>
       <c r="B67" s="9"/>
     </row>
     <row r="68" spans="1:2" ht="26" customHeight="1">
@@ -923,6 +943,9 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="26" customHeight="1">
+      <c r="A79" s="2">
+        <v>7</v>
+      </c>
       <c r="B79" s="11" t="s">
         <v>28</v>
       </c>
@@ -972,6 +995,9 @@
       <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:2" ht="26" customHeight="1">
+      <c r="A91" s="2">
+        <v>10</v>
+      </c>
       <c r="B91" s="9"/>
     </row>
     <row r="92" spans="1:2" ht="26" customHeight="1">
@@ -1017,6 +1043,9 @@
       <c r="B102" s="8"/>
     </row>
     <row r="103" spans="1:2" ht="26" customHeight="1">
+      <c r="A103" s="2">
+        <v>10</v>
+      </c>
       <c r="B103" s="9"/>
     </row>
     <row r="104" spans="1:2" ht="26" customHeight="1">
@@ -1064,6 +1093,9 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="26" customHeight="1">
+      <c r="A115" s="2">
+        <v>9</v>
+      </c>
       <c r="B115" s="9"/>
     </row>
     <row r="116" spans="1:2" ht="26" customHeight="1">
@@ -1111,6 +1143,9 @@
       </c>
     </row>
     <row r="127" spans="1:2" ht="26" customHeight="1">
+      <c r="A127" s="2">
+        <v>9</v>
+      </c>
       <c r="B127" s="9"/>
     </row>
     <row r="128" spans="1:2" ht="26" customHeight="1">
@@ -1158,6 +1193,9 @@
       </c>
     </row>
     <row r="139" spans="1:2" ht="26" customHeight="1">
+      <c r="A139" s="2">
+        <v>8</v>
+      </c>
       <c r="B139" s="11" t="s">
         <v>43</v>
       </c>

</xml_diff>